<commit_message>
Remove jk - escape combo
</commit_message>
<xml_diff>
--- a/keyboards/kyria/keymaps/kyria-luke/combos.xlsx
+++ b/keyboards/kyria/keymaps/kyria-luke/combos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\qmk_firmware\keyboards\kyria\keymaps\kyria-luke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123F6A5-7007-497F-A0E7-54A7D4B10D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91861BD4-2ABF-4B45-80C2-540D4F5D3E98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actions" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId7"/>
-    <pivotCache cacheId="21" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="439">
   <si>
     <t>Name</t>
   </si>
@@ -2347,7 +2347,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="DataPilot2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="DataPilot2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
   <location ref="A4:C55" firstHeaderRow="1" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3119,7 +3119,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000000000000}" name="DataPilot1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000000000000}" name="DataPilot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
   <location ref="A4:A26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3334,9 +3334,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="__Anonymous_Sheet_DB__2" displayName="__Anonymous_Sheet_DB__2" ref="A1:F84" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
-    <sortCondition ref="A1:A84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="__Anonymous_Sheet_DB__2" displayName="__Anonymous_Sheet_DB__2" ref="A1:F83" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E83">
+    <sortCondition ref="A1:A83"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
@@ -5005,10 +5005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:ALL85"/>
+  <dimension ref="A1:ALL84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6210,10 +6210,13 @@
         <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>207</v>
+        <v>189</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -6221,76 +6224,73 @@
         <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>308</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>308</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>182</v>
@@ -6298,10 +6298,13 @@
       <c r="C23" s="3" t="s">
         <v>202</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>182</v>
@@ -6310,32 +6313,29 @@
         <v>202</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>110</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -6343,7 +6343,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>154</v>
@@ -6351,87 +6351,76 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="4"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -8953,15 +8942,15 @@
       </c>
       <c r="C30" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C30)/2)-1,0)</f>
-        <v>j</v>
+        <v>w</v>
       </c>
       <c r="D30" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D30)/2)-1,0)</f>
-        <v>k</v>
-      </c>
-      <c r="E30" s="3">
+        <v>e</v>
+      </c>
+      <c r="E30" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E30)/2)-1,0)</f>
-        <v>0</v>
+        <v>r</v>
       </c>
       <c r="F30" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F30)/2)-1,0)</f>
@@ -8969,15 +8958,15 @@
       </c>
       <c r="G30" t="str">
         <f ca="1">VLOOKUP(C30,keys!$A$2:$C$196,$A30+1,0)</f>
-        <v>KC_J</v>
+        <v>KC_W</v>
       </c>
       <c r="H30" t="str">
         <f ca="1">VLOOKUP(D30,keys!$A$2:$C$196,$A30+1,0)</f>
-        <v>KC_K</v>
-      </c>
-      <c r="I30" t="e">
+        <v>KC_E</v>
+      </c>
+      <c r="I30" t="str">
         <f ca="1">VLOOKUP(E30,keys!$A$2:$C$196,$A30+1,0)</f>
-        <v>#N/A</v>
+        <v>KC_R</v>
       </c>
       <c r="J30" t="e">
         <f ca="1">VLOOKUP(F30,keys!$A$2:$C$196,$A30+1,0)</f>
@@ -8985,11 +8974,11 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>j_k_1</v>
+        <v>w_e_r_1</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_J, KC_K</v>
+        <v>KC_W, KC_E, KC_R</v>
       </c>
       <c r="M30" t="str">
         <f ca="1">VLOOKUP(B30,actions!$A$2:$F$514,5,0)</f>
@@ -9013,15 +9002,15 @@
       </c>
       <c r="R30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM j_k_1_combo[] = {KC_J, KC_K, COMBO_END};</v>
+        <v>const uint16_t PROGMEM w_e_r_1_combo[] = {KC_W, KC_E, KC_R, COMBO_END};</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_j_k_1,</v>
+        <v xml:space="preserve">  COMBO_w_e_r_1,</v>
       </c>
       <c r="T30" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_j_k_1] = COMBO(j_k_1_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_w_e_r_1] = COMBO(w_e_r_1_combo, KC_ESC),</v>
       </c>
       <c r="U30" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9039,31 +9028,31 @@
       </c>
       <c r="C31" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C31)/2)-1,0)</f>
-        <v>j</v>
+        <v>w</v>
       </c>
       <c r="D31" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D31)/2)-1,0)</f>
-        <v>k</v>
-      </c>
-      <c r="E31" s="3">
+        <v>e</v>
+      </c>
+      <c r="E31" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E31)/2)-1,0)</f>
-        <v>0</v>
+        <v>r</v>
       </c>
       <c r="F31" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F31)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G31" t="str">
+      <c r="G31">
         <f ca="1">VLOOKUP(C31,keys!$A$2:$C$196,$A31+1,0)</f>
-        <v>KC_4</v>
-      </c>
-      <c r="H31" t="str">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <f ca="1">VLOOKUP(D31,keys!$A$2:$C$196,$A31+1,0)</f>
-        <v>KC_5</v>
-      </c>
-      <c r="I31" t="e">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <f ca="1">VLOOKUP(E31,keys!$A$2:$C$196,$A31+1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J31" t="e">
         <f ca="1">VLOOKUP(F31,keys!$A$2:$C$196,$A31+1,0)</f>
@@ -9071,11 +9060,11 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>j_k_2</v>
+        <v>w_e_r_2</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_4, KC_5</v>
+        <v>0, 0, 0</v>
       </c>
       <c r="M31" t="str">
         <f ca="1">VLOOKUP(B31,actions!$A$2:$F$514,5,0)</f>
@@ -9095,19 +9084,19 @@
       </c>
       <c r="Q31" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM j_k_2_combo[] = {KC_4, KC_5, COMBO_END};</v>
+        <v>const uint16_t PROGMEM w_e_r_2_combo[] = {0, 0, 0, COMBO_END};</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_j_k_2,</v>
+        <v xml:space="preserve">  COMBO_w_e_r_2,</v>
       </c>
       <c r="T31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_j_k_2] = COMBO(j_k_2_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_w_e_r_2] = COMBO(w_e_r_2_combo, KC_ESC),</v>
       </c>
       <c r="U31" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9125,15 +9114,15 @@
       </c>
       <c r="C32" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C32)/2)-1,0)</f>
-        <v>w</v>
+        <v>u</v>
       </c>
       <c r="D32" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D32)/2)-1,0)</f>
-        <v>e</v>
+        <v>i</v>
       </c>
       <c r="E32" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E32)/2)-1,0)</f>
-        <v>r</v>
+        <v>o</v>
       </c>
       <c r="F32" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F32)/2)-1,0)</f>
@@ -9141,15 +9130,15 @@
       </c>
       <c r="G32" t="str">
         <f ca="1">VLOOKUP(C32,keys!$A$2:$C$196,$A32+1,0)</f>
-        <v>KC_W</v>
+        <v>KC_U</v>
       </c>
       <c r="H32" t="str">
         <f ca="1">VLOOKUP(D32,keys!$A$2:$C$196,$A32+1,0)</f>
-        <v>KC_E</v>
+        <v>KC_I</v>
       </c>
       <c r="I32" t="str">
         <f ca="1">VLOOKUP(E32,keys!$A$2:$C$196,$A32+1,0)</f>
-        <v>KC_R</v>
+        <v>KC_O</v>
       </c>
       <c r="J32" t="e">
         <f ca="1">VLOOKUP(F32,keys!$A$2:$C$196,$A32+1,0)</f>
@@ -9157,11 +9146,11 @@
       </c>
       <c r="K32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>w_e_r_1</v>
+        <v>u_i_o_1</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_W, KC_E, KC_R</v>
+        <v>KC_U, KC_I, KC_O</v>
       </c>
       <c r="M32" t="str">
         <f ca="1">VLOOKUP(B32,actions!$A$2:$F$514,5,0)</f>
@@ -9185,15 +9174,15 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM w_e_r_1_combo[] = {KC_W, KC_E, KC_R, COMBO_END};</v>
+        <v>const uint16_t PROGMEM u_i_o_1_combo[] = {KC_U, KC_I, KC_O, COMBO_END};</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_w_e_r_1,</v>
+        <v xml:space="preserve">  COMBO_u_i_o_1,</v>
       </c>
       <c r="T32" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_w_e_r_1] = COMBO(w_e_r_1_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_u_i_o_1] = COMBO(u_i_o_1_combo, KC_ESC),</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9211,31 +9200,31 @@
       </c>
       <c r="C33" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C33)/2)-1,0)</f>
-        <v>w</v>
+        <v>u</v>
       </c>
       <c r="D33" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D33)/2)-1,0)</f>
-        <v>e</v>
+        <v>i</v>
       </c>
       <c r="E33" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E33)/2)-1,0)</f>
-        <v>r</v>
+        <v>o</v>
       </c>
       <c r="F33" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F33)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="str">
         <f ca="1">VLOOKUP(C33,keys!$A$2:$C$196,$A33+1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H33">
+        <v>KC_7</v>
+      </c>
+      <c r="H33" t="str">
         <f ca="1">VLOOKUP(D33,keys!$A$2:$C$196,$A33+1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I33">
+        <v>KC_8</v>
+      </c>
+      <c r="I33" t="str">
         <f ca="1">VLOOKUP(E33,keys!$A$2:$C$196,$A33+1,0)</f>
-        <v>0</v>
+        <v>KC_9</v>
       </c>
       <c r="J33" t="e">
         <f ca="1">VLOOKUP(F33,keys!$A$2:$C$196,$A33+1,0)</f>
@@ -9243,11 +9232,11 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>w_e_r_2</v>
+        <v>u_i_o_2</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0, 0, 0</v>
+        <v>KC_7, KC_8, KC_9</v>
       </c>
       <c r="M33" t="str">
         <f ca="1">VLOOKUP(B33,actions!$A$2:$F$514,5,0)</f>
@@ -9267,19 +9256,19 @@
       </c>
       <c r="Q33" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM w_e_r_2_combo[] = {0, 0, 0, COMBO_END};</v>
+        <v>const uint16_t PROGMEM u_i_o_2_combo[] = {KC_7, KC_8, KC_9, COMBO_END};</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_w_e_r_2,</v>
+        <v xml:space="preserve">  COMBO_u_i_o_2,</v>
       </c>
       <c r="T33" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_w_e_r_2] = COMBO(w_e_r_2_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_u_i_o_2] = COMBO(u_i_o_2_combo, KC_ESC),</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9293,19 +9282,19 @@
       </c>
       <c r="B34" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B34)/2)-1,0)</f>
-        <v>esc</v>
+        <v>macro_play</v>
       </c>
       <c r="C34" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C34)/2)-1,0)</f>
-        <v>u</v>
+        <v>q</v>
       </c>
       <c r="D34" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D34)/2)-1,0)</f>
-        <v>i</v>
-      </c>
-      <c r="E34" s="3" t="str">
+        <v>w</v>
+      </c>
+      <c r="E34" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E34)/2)-1,0)</f>
-        <v>o</v>
+        <v>0</v>
       </c>
       <c r="F34" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F34)/2)-1,0)</f>
@@ -9313,15 +9302,15 @@
       </c>
       <c r="G34" t="str">
         <f ca="1">VLOOKUP(C34,keys!$A$2:$C$196,$A34+1,0)</f>
-        <v>KC_U</v>
+        <v>KC_Q</v>
       </c>
       <c r="H34" t="str">
         <f ca="1">VLOOKUP(D34,keys!$A$2:$C$196,$A34+1,0)</f>
-        <v>KC_I</v>
-      </c>
-      <c r="I34" t="str">
+        <v>KC_W</v>
+      </c>
+      <c r="I34" t="e">
         <f ca="1">VLOOKUP(E34,keys!$A$2:$C$196,$A34+1,0)</f>
-        <v>KC_O</v>
+        <v>#N/A</v>
       </c>
       <c r="J34" t="e">
         <f ca="1">VLOOKUP(F34,keys!$A$2:$C$196,$A34+1,0)</f>
@@ -9329,11 +9318,11 @@
       </c>
       <c r="K34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>u_i_o_1</v>
+        <v>q_w_1</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_U, KC_I, KC_O</v>
+        <v>KC_Q, KC_W</v>
       </c>
       <c r="M34" t="str">
         <f ca="1">VLOOKUP(B34,actions!$A$2:$F$514,5,0)</f>
@@ -9341,7 +9330,7 @@
       </c>
       <c r="N34" t="str">
         <f ca="1">VLOOKUP(B34,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_ESC</v>
+        <v>DYN_MACRO_PLAY1</v>
       </c>
       <c r="O34">
         <f ca="1">VLOOKUP(B34,actions!$A$2:$D$514,3,0)</f>
@@ -9357,15 +9346,15 @@
       </c>
       <c r="R34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM u_i_o_1_combo[] = {KC_U, KC_I, KC_O, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_w_1_combo[] = {KC_Q, KC_W, COMBO_END};</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_u_i_o_1,</v>
+        <v xml:space="preserve">  COMBO_q_w_1,</v>
       </c>
       <c r="T34" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_u_i_o_1] = COMBO(u_i_o_1_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_q_w_1] = COMBO(q_w_1_combo, DYN_MACRO_PLAY1),</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9379,35 +9368,35 @@
       </c>
       <c r="B35" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B35)/2)-1,0)</f>
-        <v>esc</v>
+        <v>macro_play</v>
       </c>
       <c r="C35" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C35)/2)-1,0)</f>
-        <v>u</v>
+        <v>q</v>
       </c>
       <c r="D35" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D35)/2)-1,0)</f>
-        <v>i</v>
-      </c>
-      <c r="E35" s="3" t="str">
+        <v>w</v>
+      </c>
+      <c r="E35" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E35)/2)-1,0)</f>
-        <v>o</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F35)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G35" t="str">
+      <c r="G35">
         <f ca="1">VLOOKUP(C35,keys!$A$2:$C$196,$A35+1,0)</f>
-        <v>KC_7</v>
-      </c>
-      <c r="H35" t="str">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <f ca="1">VLOOKUP(D35,keys!$A$2:$C$196,$A35+1,0)</f>
-        <v>KC_8</v>
-      </c>
-      <c r="I35" t="str">
+        <v>0</v>
+      </c>
+      <c r="I35" t="e">
         <f ca="1">VLOOKUP(E35,keys!$A$2:$C$196,$A35+1,0)</f>
-        <v>KC_9</v>
+        <v>#N/A</v>
       </c>
       <c r="J35" t="e">
         <f ca="1">VLOOKUP(F35,keys!$A$2:$C$196,$A35+1,0)</f>
@@ -9415,11 +9404,11 @@
       </c>
       <c r="K35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>u_i_o_2</v>
+        <v>q_w_2</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_7, KC_8, KC_9</v>
+        <v>0, 0</v>
       </c>
       <c r="M35" t="str">
         <f ca="1">VLOOKUP(B35,actions!$A$2:$F$514,5,0)</f>
@@ -9427,7 +9416,7 @@
       </c>
       <c r="N35" t="str">
         <f ca="1">VLOOKUP(B35,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_ESC</v>
+        <v>DYN_MACRO_PLAY1</v>
       </c>
       <c r="O35">
         <f ca="1">VLOOKUP(B35,actions!$A$2:$D$514,3,0)</f>
@@ -9439,19 +9428,19 @@
       </c>
       <c r="Q35" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM u_i_o_2_combo[] = {KC_7, KC_8, KC_9, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_w_2_combo[] = {0, 0, COMBO_END};</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_u_i_o_2,</v>
+        <v xml:space="preserve">  COMBO_q_w_2,</v>
       </c>
       <c r="T35" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_u_i_o_2] = COMBO(u_i_o_2_combo, KC_ESC),</v>
+        <v xml:space="preserve">  [COMBO_q_w_2] = COMBO(q_w_2_combo, DYN_MACRO_PLAY1),</v>
       </c>
       <c r="U35" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9465,7 +9454,7 @@
       </c>
       <c r="B36" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B36)/2)-1,0)</f>
-        <v>macro_play</v>
+        <v>macro_rec</v>
       </c>
       <c r="C36" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C36)/2)-1,0)</f>
@@ -9473,7 +9462,7 @@
       </c>
       <c r="D36" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D36)/2)-1,0)</f>
-        <v>w</v>
+        <v>r</v>
       </c>
       <c r="E36" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E36)/2)-1,0)</f>
@@ -9489,7 +9478,7 @@
       </c>
       <c r="H36" t="str">
         <f ca="1">VLOOKUP(D36,keys!$A$2:$C$196,$A36+1,0)</f>
-        <v>KC_W</v>
+        <v>KC_R</v>
       </c>
       <c r="I36" t="e">
         <f ca="1">VLOOKUP(E36,keys!$A$2:$C$196,$A36+1,0)</f>
@@ -9501,11 +9490,11 @@
       </c>
       <c r="K36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_w_1</v>
+        <v>q_r_1</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_Q, KC_W</v>
+        <v>KC_Q, KC_R</v>
       </c>
       <c r="M36" t="str">
         <f ca="1">VLOOKUP(B36,actions!$A$2:$F$514,5,0)</f>
@@ -9513,7 +9502,7 @@
       </c>
       <c r="N36" t="str">
         <f ca="1">VLOOKUP(B36,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_MACRO_PLAY1</v>
+        <v>DYN_REC_START1</v>
       </c>
       <c r="O36">
         <f ca="1">VLOOKUP(B36,actions!$A$2:$D$514,3,0)</f>
@@ -9529,15 +9518,15 @@
       </c>
       <c r="R36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_w_1_combo[] = {KC_Q, KC_W, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_r_1_combo[] = {KC_Q, KC_R, COMBO_END};</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_w_1,</v>
+        <v xml:space="preserve">  COMBO_q_r_1,</v>
       </c>
       <c r="T36" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_w_1] = COMBO(q_w_1_combo, DYN_MACRO_PLAY1),</v>
+        <v xml:space="preserve">  [COMBO_q_r_1] = COMBO(q_r_1_combo, DYN_REC_START1),</v>
       </c>
       <c r="U36" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9551,7 +9540,7 @@
       </c>
       <c r="B37" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B37)/2)-1,0)</f>
-        <v>macro_play</v>
+        <v>macro_rec</v>
       </c>
       <c r="C37" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C37)/2)-1,0)</f>
@@ -9559,7 +9548,7 @@
       </c>
       <c r="D37" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D37)/2)-1,0)</f>
-        <v>w</v>
+        <v>r</v>
       </c>
       <c r="E37" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E37)/2)-1,0)</f>
@@ -9587,7 +9576,7 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_w_2</v>
+        <v>q_r_2</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -9599,7 +9588,7 @@
       </c>
       <c r="N37" t="str">
         <f ca="1">VLOOKUP(B37,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_MACRO_PLAY1</v>
+        <v>DYN_REC_START1</v>
       </c>
       <c r="O37">
         <f ca="1">VLOOKUP(B37,actions!$A$2:$D$514,3,0)</f>
@@ -9615,15 +9604,15 @@
       </c>
       <c r="R37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_w_2_combo[] = {0, 0, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_r_2_combo[] = {0, 0, COMBO_END};</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_w_2,</v>
+        <v xml:space="preserve">  COMBO_q_r_2,</v>
       </c>
       <c r="T37" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_w_2] = COMBO(q_w_2_combo, DYN_MACRO_PLAY1),</v>
+        <v xml:space="preserve">  [COMBO_q_r_2] = COMBO(q_r_2_combo, DYN_REC_START1),</v>
       </c>
       <c r="U37" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9637,7 +9626,7 @@
       </c>
       <c r="B38" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B38)/2)-1,0)</f>
-        <v>macro_rec</v>
+        <v>macro_stop</v>
       </c>
       <c r="C38" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C38)/2)-1,0)</f>
@@ -9645,7 +9634,7 @@
       </c>
       <c r="D38" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D38)/2)-1,0)</f>
-        <v>r</v>
+        <v>s</v>
       </c>
       <c r="E38" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E38)/2)-1,0)</f>
@@ -9661,7 +9650,7 @@
       </c>
       <c r="H38" t="str">
         <f ca="1">VLOOKUP(D38,keys!$A$2:$C$196,$A38+1,0)</f>
-        <v>KC_R</v>
+        <v>KC_S</v>
       </c>
       <c r="I38" t="e">
         <f ca="1">VLOOKUP(E38,keys!$A$2:$C$196,$A38+1,0)</f>
@@ -9673,11 +9662,11 @@
       </c>
       <c r="K38" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_r_1</v>
+        <v>q_s_1</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_Q, KC_R</v>
+        <v>KC_Q, KC_S</v>
       </c>
       <c r="M38" t="str">
         <f ca="1">VLOOKUP(B38,actions!$A$2:$F$514,5,0)</f>
@@ -9685,7 +9674,7 @@
       </c>
       <c r="N38" t="str">
         <f ca="1">VLOOKUP(B38,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_REC_START1</v>
+        <v>DYN_REC_STOP</v>
       </c>
       <c r="O38">
         <f ca="1">VLOOKUP(B38,actions!$A$2:$D$514,3,0)</f>
@@ -9701,15 +9690,15 @@
       </c>
       <c r="R38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_r_1_combo[] = {KC_Q, KC_R, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_s_1_combo[] = {KC_Q, KC_S, COMBO_END};</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_r_1,</v>
+        <v xml:space="preserve">  COMBO_q_s_1,</v>
       </c>
       <c r="T38" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_r_1] = COMBO(q_r_1_combo, DYN_REC_START1),</v>
+        <v xml:space="preserve">  [COMBO_q_s_1] = COMBO(q_s_1_combo, DYN_REC_STOP),</v>
       </c>
       <c r="U38" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9723,7 +9712,7 @@
       </c>
       <c r="B39" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B39)/2)-1,0)</f>
-        <v>macro_rec</v>
+        <v>macro_stop</v>
       </c>
       <c r="C39" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C39)/2)-1,0)</f>
@@ -9731,7 +9720,7 @@
       </c>
       <c r="D39" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D39)/2)-1,0)</f>
-        <v>r</v>
+        <v>s</v>
       </c>
       <c r="E39" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E39)/2)-1,0)</f>
@@ -9745,9 +9734,9 @@
         <f ca="1">VLOOKUP(C39,keys!$A$2:$C$196,$A39+1,0)</f>
         <v>0</v>
       </c>
-      <c r="H39">
+      <c r="H39" t="str">
         <f ca="1">VLOOKUP(D39,keys!$A$2:$C$196,$A39+1,0)</f>
-        <v>0</v>
+        <v>KC_LPRN</v>
       </c>
       <c r="I39" t="e">
         <f ca="1">VLOOKUP(E39,keys!$A$2:$C$196,$A39+1,0)</f>
@@ -9759,11 +9748,11 @@
       </c>
       <c r="K39" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_r_2</v>
+        <v>q_s_2</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0, 0</v>
+        <v>0, KC_LPRN</v>
       </c>
       <c r="M39" t="str">
         <f ca="1">VLOOKUP(B39,actions!$A$2:$F$514,5,0)</f>
@@ -9771,7 +9760,7 @@
       </c>
       <c r="N39" t="str">
         <f ca="1">VLOOKUP(B39,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_REC_START1</v>
+        <v>DYN_REC_STOP</v>
       </c>
       <c r="O39">
         <f ca="1">VLOOKUP(B39,actions!$A$2:$D$514,3,0)</f>
@@ -9787,15 +9776,15 @@
       </c>
       <c r="R39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_r_2_combo[] = {0, 0, COMBO_END};</v>
+        <v>const uint16_t PROGMEM q_s_2_combo[] = {0, KC_LPRN, COMBO_END};</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_r_2,</v>
+        <v xml:space="preserve">  COMBO_q_s_2,</v>
       </c>
       <c r="T39" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_r_2] = COMBO(q_r_2_combo, DYN_REC_START1),</v>
+        <v xml:space="preserve">  [COMBO_q_s_2] = COMBO(q_s_2_combo, DYN_REC_STOP),</v>
       </c>
       <c r="U39" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9809,15 +9798,15 @@
       </c>
       <c r="B40" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B40)/2)-1,0)</f>
-        <v>macro_stop</v>
+        <v>menu</v>
       </c>
       <c r="C40" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C40)/2)-1,0)</f>
-        <v>q</v>
+        <v>m</v>
       </c>
       <c r="D40" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D40)/2)-1,0)</f>
-        <v>s</v>
+        <v>dot</v>
       </c>
       <c r="E40" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E40)/2)-1,0)</f>
@@ -9829,11 +9818,11 @@
       </c>
       <c r="G40" t="str">
         <f ca="1">VLOOKUP(C40,keys!$A$2:$C$196,$A40+1,0)</f>
-        <v>KC_Q</v>
+        <v>KC_M</v>
       </c>
       <c r="H40" t="str">
         <f ca="1">VLOOKUP(D40,keys!$A$2:$C$196,$A40+1,0)</f>
-        <v>KC_S</v>
+        <v>KC_DOT</v>
       </c>
       <c r="I40" t="e">
         <f ca="1">VLOOKUP(E40,keys!$A$2:$C$196,$A40+1,0)</f>
@@ -9845,11 +9834,11 @@
       </c>
       <c r="K40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_s_1</v>
+        <v>m_dot_1</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_Q, KC_S</v>
+        <v>KC_M, KC_DOT</v>
       </c>
       <c r="M40" t="str">
         <f ca="1">VLOOKUP(B40,actions!$A$2:$F$514,5,0)</f>
@@ -9857,7 +9846,7 @@
       </c>
       <c r="N40" t="str">
         <f ca="1">VLOOKUP(B40,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_REC_STOP</v>
+        <v>KC_APP</v>
       </c>
       <c r="O40">
         <f ca="1">VLOOKUP(B40,actions!$A$2:$D$514,3,0)</f>
@@ -9873,15 +9862,15 @@
       </c>
       <c r="R40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_s_1_combo[] = {KC_Q, KC_S, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_dot_1_combo[] = {KC_M, KC_DOT, COMBO_END};</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_s_1,</v>
+        <v xml:space="preserve">  COMBO_m_dot_1,</v>
       </c>
       <c r="T40" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_s_1] = COMBO(q_s_1_combo, DYN_REC_STOP),</v>
+        <v xml:space="preserve">  [COMBO_m_dot_1] = COMBO(m_dot_1_combo, KC_APP),</v>
       </c>
       <c r="U40" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9895,15 +9884,15 @@
       </c>
       <c r="B41" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B41)/2)-1,0)</f>
-        <v>macro_stop</v>
+        <v>menu</v>
       </c>
       <c r="C41" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C41)/2)-1,0)</f>
-        <v>q</v>
+        <v>m</v>
       </c>
       <c r="D41" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D41)/2)-1,0)</f>
-        <v>s</v>
+        <v>dot</v>
       </c>
       <c r="E41" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E41)/2)-1,0)</f>
@@ -9913,13 +9902,13 @@
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F41)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G41">
+      <c r="G41" t="str">
         <f ca="1">VLOOKUP(C41,keys!$A$2:$C$196,$A41+1,0)</f>
-        <v>0</v>
+        <v>KC_1</v>
       </c>
       <c r="H41" t="str">
         <f ca="1">VLOOKUP(D41,keys!$A$2:$C$196,$A41+1,0)</f>
-        <v>KC_LPRN</v>
+        <v>KC_3</v>
       </c>
       <c r="I41" t="e">
         <f ca="1">VLOOKUP(E41,keys!$A$2:$C$196,$A41+1,0)</f>
@@ -9931,11 +9920,11 @@
       </c>
       <c r="K41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>q_s_2</v>
+        <v>m_dot_2</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0, KC_LPRN</v>
+        <v>KC_1, KC_3</v>
       </c>
       <c r="M41" t="str">
         <f ca="1">VLOOKUP(B41,actions!$A$2:$F$514,5,0)</f>
@@ -9943,7 +9932,7 @@
       </c>
       <c r="N41" t="str">
         <f ca="1">VLOOKUP(B41,actions!$A$2:$D$514,2,0)</f>
-        <v>DYN_REC_STOP</v>
+        <v>KC_APP</v>
       </c>
       <c r="O41">
         <f ca="1">VLOOKUP(B41,actions!$A$2:$D$514,3,0)</f>
@@ -9955,19 +9944,19 @@
       </c>
       <c r="Q41" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM q_s_2_combo[] = {0, KC_LPRN, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_dot_2_combo[] = {KC_1, KC_3, COMBO_END};</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_q_s_2,</v>
+        <v xml:space="preserve">  COMBO_m_dot_2,</v>
       </c>
       <c r="T41" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_q_s_2] = COMBO(q_s_2_combo, DYN_REC_STOP),</v>
+        <v xml:space="preserve">  [COMBO_m_dot_2] = COMBO(m_dot_2_combo, KC_APP),</v>
       </c>
       <c r="U41" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -9981,15 +9970,15 @@
       </c>
       <c r="B42" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B42)/2)-1,0)</f>
-        <v>menu</v>
+        <v>paste</v>
       </c>
       <c r="C42" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C42)/2)-1,0)</f>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="D42" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D42)/2)-1,0)</f>
-        <v>dot</v>
+        <v>v</v>
       </c>
       <c r="E42" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E42)/2)-1,0)</f>
@@ -10001,11 +9990,11 @@
       </c>
       <c r="G42" t="str">
         <f ca="1">VLOOKUP(C42,keys!$A$2:$C$196,$A42+1,0)</f>
-        <v>KC_M</v>
+        <v>KC_D</v>
       </c>
       <c r="H42" t="str">
         <f ca="1">VLOOKUP(D42,keys!$A$2:$C$196,$A42+1,0)</f>
-        <v>KC_DOT</v>
+        <v>KC_V</v>
       </c>
       <c r="I42" t="e">
         <f ca="1">VLOOKUP(E42,keys!$A$2:$C$196,$A42+1,0)</f>
@@ -10017,23 +10006,23 @@
       </c>
       <c r="K42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_dot_1</v>
+        <v>d_v_1</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_M, KC_DOT</v>
+        <v>KC_D, KC_V</v>
       </c>
       <c r="M42" t="str">
         <f ca="1">VLOOKUP(B42,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N42" t="str">
+        <v>macro</v>
+      </c>
+      <c r="N42">
         <f ca="1">VLOOKUP(B42,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_APP</v>
-      </c>
-      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="str">
         <f ca="1">VLOOKUP(B42,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
+        <v>tap_code16(RSFT(KC_INS));</v>
       </c>
       <c r="P42">
         <f ca="1">VLOOKUP(B42,actions!$A$2:$D$514,4,0)</f>
@@ -10045,19 +10034,19 @@
       </c>
       <c r="R42" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_dot_1_combo[] = {KC_M, KC_DOT, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_1_combo[] = {KC_D, KC_V, COMBO_END};</v>
       </c>
       <c r="S42" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_dot_1,</v>
+        <v xml:space="preserve">  COMBO_d_v_1,</v>
       </c>
       <c r="T42" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_dot_1] = COMBO(m_dot_1_combo, KC_APP),</v>
+        <v xml:space="preserve">  [COMBO_d_v_1] = COMBO_ACTION(d_v_1_combo),</v>
       </c>
       <c r="U42" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v xml:space="preserve">    case COMBO_d_v_1: if (p) {tap_code16(RSFT(KC_INS));}  break;</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -10067,15 +10056,15 @@
       </c>
       <c r="B43" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B43)/2)-1,0)</f>
-        <v>menu</v>
+        <v>paste</v>
       </c>
       <c r="C43" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C43)/2)-1,0)</f>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="D43" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D43)/2)-1,0)</f>
-        <v>dot</v>
+        <v>v</v>
       </c>
       <c r="E43" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E43)/2)-1,0)</f>
@@ -10087,11 +10076,11 @@
       </c>
       <c r="G43" t="str">
         <f ca="1">VLOOKUP(C43,keys!$A$2:$C$196,$A43+1,0)</f>
-        <v>KC_1</v>
-      </c>
-      <c r="H43" t="str">
+        <v>KC_LPRN</v>
+      </c>
+      <c r="H43">
         <f ca="1">VLOOKUP(D43,keys!$A$2:$C$196,$A43+1,0)</f>
-        <v>KC_3</v>
+        <v>0</v>
       </c>
       <c r="I43" t="e">
         <f ca="1">VLOOKUP(E43,keys!$A$2:$C$196,$A43+1,0)</f>
@@ -10103,23 +10092,23 @@
       </c>
       <c r="K43" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_dot_2</v>
+        <v>d_v_2</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_1, KC_3</v>
+        <v>KC_LPRN, 0</v>
       </c>
       <c r="M43" t="str">
         <f ca="1">VLOOKUP(B43,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N43" t="str">
+        <v>macro</v>
+      </c>
+      <c r="N43">
         <f ca="1">VLOOKUP(B43,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_APP</v>
-      </c>
-      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="str">
         <f ca="1">VLOOKUP(B43,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
+        <v>tap_code16(RSFT(KC_INS));</v>
       </c>
       <c r="P43">
         <f ca="1">VLOOKUP(B43,actions!$A$2:$D$514,4,0)</f>
@@ -10127,23 +10116,23 @@
       </c>
       <c r="Q43" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R43" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_dot_2_combo[] = {KC_1, KC_3, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_2_combo[] = {KC_LPRN, 0, COMBO_END};</v>
       </c>
       <c r="S43" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_dot_2,</v>
+        <v xml:space="preserve">  COMBO_d_v_2,</v>
       </c>
       <c r="T43" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_dot_2] = COMBO(m_dot_2_combo, KC_APP),</v>
+        <v xml:space="preserve">  [COMBO_d_v_2] = COMBO_ACTION(d_v_2_combo),</v>
       </c>
       <c r="U43" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v xml:space="preserve">    case COMBO_d_v_2: if (p) {tap_code16(RSFT(KC_INS));}  break;</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -10153,7 +10142,7 @@
       </c>
       <c r="B44" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B44)/2)-1,0)</f>
-        <v>paste</v>
+        <v>paste_all</v>
       </c>
       <c r="C44" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C44)/2)-1,0)</f>
@@ -10163,9 +10152,9 @@
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D44)/2)-1,0)</f>
         <v>v</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E44)/2)-1,0)</f>
-        <v>0</v>
+        <v>a</v>
       </c>
       <c r="F44" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F44)/2)-1,0)</f>
@@ -10179,9 +10168,9 @@
         <f ca="1">VLOOKUP(D44,keys!$A$2:$C$196,$A44+1,0)</f>
         <v>KC_V</v>
       </c>
-      <c r="I44" t="e">
+      <c r="I44" t="str">
         <f ca="1">VLOOKUP(E44,keys!$A$2:$C$196,$A44+1,0)</f>
-        <v>#N/A</v>
+        <v>KC_A</v>
       </c>
       <c r="J44" t="e">
         <f ca="1">VLOOKUP(F44,keys!$A$2:$C$196,$A44+1,0)</f>
@@ -10189,11 +10178,11 @@
       </c>
       <c r="K44" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_1</v>
+        <v>d_v_a_1</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_D, KC_V</v>
+        <v>KC_D, KC_V, KC_A</v>
       </c>
       <c r="M44" t="str">
         <f ca="1">VLOOKUP(B44,actions!$A$2:$F$514,5,0)</f>
@@ -10205,7 +10194,7 @@
       </c>
       <c r="O44" t="str">
         <f ca="1">VLOOKUP(B44,actions!$A$2:$D$514,3,0)</f>
-        <v>tap_code16(RSFT(KC_INS));</v>
+        <v>SEND_STRING(SS_RCTL("av"));</v>
       </c>
       <c r="P44">
         <f ca="1">VLOOKUP(B44,actions!$A$2:$D$514,4,0)</f>
@@ -10217,19 +10206,19 @@
       </c>
       <c r="R44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_1_combo[] = {KC_D, KC_V, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_a_1_combo[] = {KC_D, KC_V, KC_A, COMBO_END};</v>
       </c>
       <c r="S44" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_1,</v>
+        <v xml:space="preserve">  COMBO_d_v_a_1,</v>
       </c>
       <c r="T44" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_1] = COMBO_ACTION(d_v_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_d_v_a_1] = COMBO_ACTION(d_v_a_1_combo),</v>
       </c>
       <c r="U44" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_1: if (p) {tap_code16(RSFT(KC_INS));}  break;</v>
+        <v xml:space="preserve">    case COMBO_d_v_a_1: if (p) {SEND_STRING(SS_RCTL("av"));}  break;</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -10239,7 +10228,7 @@
       </c>
       <c r="B45" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B45)/2)-1,0)</f>
-        <v>paste</v>
+        <v>paste_all</v>
       </c>
       <c r="C45" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C45)/2)-1,0)</f>
@@ -10249,9 +10238,9 @@
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D45)/2)-1,0)</f>
         <v>v</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E45)/2)-1,0)</f>
-        <v>0</v>
+        <v>a</v>
       </c>
       <c r="F45" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F45)/2)-1,0)</f>
@@ -10265,9 +10254,9 @@
         <f ca="1">VLOOKUP(D45,keys!$A$2:$C$196,$A45+1,0)</f>
         <v>0</v>
       </c>
-      <c r="I45" t="e">
+      <c r="I45" t="str">
         <f ca="1">VLOOKUP(E45,keys!$A$2:$C$196,$A45+1,0)</f>
-        <v>#N/A</v>
+        <v>KC_LBRC</v>
       </c>
       <c r="J45" t="e">
         <f ca="1">VLOOKUP(F45,keys!$A$2:$C$196,$A45+1,0)</f>
@@ -10275,11 +10264,11 @@
       </c>
       <c r="K45" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_2</v>
+        <v>d_v_a_2</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, 0</v>
+        <v>KC_LPRN, 0, KC_LBRC</v>
       </c>
       <c r="M45" t="str">
         <f ca="1">VLOOKUP(B45,actions!$A$2:$F$514,5,0)</f>
@@ -10291,7 +10280,7 @@
       </c>
       <c r="O45" t="str">
         <f ca="1">VLOOKUP(B45,actions!$A$2:$D$514,3,0)</f>
-        <v>tap_code16(RSFT(KC_INS));</v>
+        <v>SEND_STRING(SS_RCTL("av"));</v>
       </c>
       <c r="P45">
         <f ca="1">VLOOKUP(B45,actions!$A$2:$D$514,4,0)</f>
@@ -10303,19 +10292,19 @@
       </c>
       <c r="R45" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_2_combo[] = {KC_LPRN, 0, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_a_2_combo[] = {KC_LPRN, 0, KC_LBRC, COMBO_END};</v>
       </c>
       <c r="S45" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_2,</v>
+        <v xml:space="preserve">  COMBO_d_v_a_2,</v>
       </c>
       <c r="T45" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_2] = COMBO_ACTION(d_v_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_d_v_a_2] = COMBO_ACTION(d_v_a_2_combo),</v>
       </c>
       <c r="U45" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_2: if (p) {tap_code16(RSFT(KC_INS));}  break;</v>
+        <v xml:space="preserve">    case COMBO_d_v_a_2: if (p) {SEND_STRING(SS_RCTL("av"));}  break;</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -10325,7 +10314,7 @@
       </c>
       <c r="B46" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B46)/2)-1,0)</f>
-        <v>paste_all</v>
+        <v>paste_ditto</v>
       </c>
       <c r="C46" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C46)/2)-1,0)</f>
@@ -10337,7 +10326,7 @@
       </c>
       <c r="E46" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E46)/2)-1,0)</f>
-        <v>a</v>
+        <v>s</v>
       </c>
       <c r="F46" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F46)/2)-1,0)</f>
@@ -10353,7 +10342,7 @@
       </c>
       <c r="I46" t="str">
         <f ca="1">VLOOKUP(E46,keys!$A$2:$C$196,$A46+1,0)</f>
-        <v>KC_A</v>
+        <v>KC_S</v>
       </c>
       <c r="J46" t="e">
         <f ca="1">VLOOKUP(F46,keys!$A$2:$C$196,$A46+1,0)</f>
@@ -10361,11 +10350,11 @@
       </c>
       <c r="K46" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_a_1</v>
+        <v>d_v_s_1</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_D, KC_V, KC_A</v>
+        <v>KC_D, KC_V, KC_S</v>
       </c>
       <c r="M46" t="str">
         <f ca="1">VLOOKUP(B46,actions!$A$2:$F$514,5,0)</f>
@@ -10377,7 +10366,7 @@
       </c>
       <c r="O46" t="str">
         <f ca="1">VLOOKUP(B46,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("av"));</v>
+        <v>SEND_STRING(SS_RGUI("`"));</v>
       </c>
       <c r="P46">
         <f ca="1">VLOOKUP(B46,actions!$A$2:$D$514,4,0)</f>
@@ -10389,19 +10378,19 @@
       </c>
       <c r="R46" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_a_1_combo[] = {KC_D, KC_V, KC_A, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_s_1_combo[] = {KC_D, KC_V, KC_S, COMBO_END};</v>
       </c>
       <c r="S46" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_a_1,</v>
+        <v xml:space="preserve">  COMBO_d_v_s_1,</v>
       </c>
       <c r="T46" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_a_1] = COMBO_ACTION(d_v_a_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_d_v_s_1] = COMBO_ACTION(d_v_s_1_combo),</v>
       </c>
       <c r="U46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_a_1: if (p) {SEND_STRING(SS_RCTL("av"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_d_v_s_1: if (p) {SEND_STRING(SS_RGUI("`"));}  break;</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -10411,7 +10400,7 @@
       </c>
       <c r="B47" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B47)/2)-1,0)</f>
-        <v>paste_all</v>
+        <v>paste_ditto</v>
       </c>
       <c r="C47" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C47)/2)-1,0)</f>
@@ -10423,7 +10412,7 @@
       </c>
       <c r="E47" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E47)/2)-1,0)</f>
-        <v>a</v>
+        <v>s</v>
       </c>
       <c r="F47" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F47)/2)-1,0)</f>
@@ -10439,7 +10428,7 @@
       </c>
       <c r="I47" t="str">
         <f ca="1">VLOOKUP(E47,keys!$A$2:$C$196,$A47+1,0)</f>
-        <v>KC_LBRC</v>
+        <v>KC_LPRN</v>
       </c>
       <c r="J47" t="e">
         <f ca="1">VLOOKUP(F47,keys!$A$2:$C$196,$A47+1,0)</f>
@@ -10447,11 +10436,11 @@
       </c>
       <c r="K47" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_a_2</v>
+        <v>d_v_s_2</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, 0, KC_LBRC</v>
+        <v>KC_LPRN, 0, KC_LPRN</v>
       </c>
       <c r="M47" t="str">
         <f ca="1">VLOOKUP(B47,actions!$A$2:$F$514,5,0)</f>
@@ -10463,7 +10452,7 @@
       </c>
       <c r="O47" t="str">
         <f ca="1">VLOOKUP(B47,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("av"));</v>
+        <v>SEND_STRING(SS_RGUI("`"));</v>
       </c>
       <c r="P47">
         <f ca="1">VLOOKUP(B47,actions!$A$2:$D$514,4,0)</f>
@@ -10475,19 +10464,19 @@
       </c>
       <c r="R47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_a_2_combo[] = {KC_LPRN, 0, KC_LBRC, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_v_s_2_combo[] = {KC_LPRN, 0, KC_LPRN, COMBO_END};</v>
       </c>
       <c r="S47" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_a_2,</v>
+        <v xml:space="preserve">  COMBO_d_v_s_2,</v>
       </c>
       <c r="T47" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_a_2] = COMBO_ACTION(d_v_a_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_d_v_s_2] = COMBO_ACTION(d_v_s_2_combo),</v>
       </c>
       <c r="U47" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_a_2: if (p) {SEND_STRING(SS_RCTL("av"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_d_v_s_2: if (p) {SEND_STRING(SS_RGUI("`"));}  break;</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -10497,19 +10486,19 @@
       </c>
       <c r="B48" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B48)/2)-1,0)</f>
-        <v>paste_ditto</v>
+        <v>save</v>
       </c>
       <c r="C48" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C48)/2)-1,0)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="D48" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D48)/2)-1,0)</f>
         <v>v</v>
       </c>
-      <c r="E48" s="3" t="str">
+      <c r="E48" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E48)/2)-1,0)</f>
-        <v>s</v>
+        <v>0</v>
       </c>
       <c r="F48" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F48)/2)-1,0)</f>
@@ -10517,15 +10506,15 @@
       </c>
       <c r="G48" t="str">
         <f ca="1">VLOOKUP(C48,keys!$A$2:$C$196,$A48+1,0)</f>
-        <v>KC_D</v>
+        <v>KC_S</v>
       </c>
       <c r="H48" t="str">
         <f ca="1">VLOOKUP(D48,keys!$A$2:$C$196,$A48+1,0)</f>
         <v>KC_V</v>
       </c>
-      <c r="I48" t="str">
+      <c r="I48" t="e">
         <f ca="1">VLOOKUP(E48,keys!$A$2:$C$196,$A48+1,0)</f>
-        <v>KC_S</v>
+        <v>#N/A</v>
       </c>
       <c r="J48" t="e">
         <f ca="1">VLOOKUP(F48,keys!$A$2:$C$196,$A48+1,0)</f>
@@ -10533,11 +10522,11 @@
       </c>
       <c r="K48" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_s_1</v>
+        <v>s_v_1</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_D, KC_V, KC_S</v>
+        <v>KC_S, KC_V</v>
       </c>
       <c r="M48" t="str">
         <f ca="1">VLOOKUP(B48,actions!$A$2:$F$514,5,0)</f>
@@ -10549,7 +10538,7 @@
       </c>
       <c r="O48" t="str">
         <f ca="1">VLOOKUP(B48,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RGUI("`"));</v>
+        <v>SEND_STRING(SS_RCTL("s"));</v>
       </c>
       <c r="P48">
         <f ca="1">VLOOKUP(B48,actions!$A$2:$D$514,4,0)</f>
@@ -10561,19 +10550,19 @@
       </c>
       <c r="R48" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_s_1_combo[] = {KC_D, KC_V, KC_S, COMBO_END};</v>
+        <v>const uint16_t PROGMEM s_v_1_combo[] = {KC_S, KC_V, COMBO_END};</v>
       </c>
       <c r="S48" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_s_1,</v>
+        <v xml:space="preserve">  COMBO_s_v_1,</v>
       </c>
       <c r="T48" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_s_1] = COMBO_ACTION(d_v_s_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_s_v_1] = COMBO_ACTION(s_v_1_combo),</v>
       </c>
       <c r="U48" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_s_1: if (p) {SEND_STRING(SS_RGUI("`"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_s_v_1: if (p) {SEND_STRING(SS_RCTL("s"));}  break;</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -10583,19 +10572,19 @@
       </c>
       <c r="B49" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B49)/2)-1,0)</f>
-        <v>paste_ditto</v>
+        <v>save</v>
       </c>
       <c r="C49" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C49)/2)-1,0)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="D49" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D49)/2)-1,0)</f>
         <v>v</v>
       </c>
-      <c r="E49" s="3" t="str">
+      <c r="E49" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E49)/2)-1,0)</f>
-        <v>s</v>
+        <v>0</v>
       </c>
       <c r="F49" s="3">
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F49)/2)-1,0)</f>
@@ -10609,9 +10598,9 @@
         <f ca="1">VLOOKUP(D49,keys!$A$2:$C$196,$A49+1,0)</f>
         <v>0</v>
       </c>
-      <c r="I49" t="str">
+      <c r="I49" t="e">
         <f ca="1">VLOOKUP(E49,keys!$A$2:$C$196,$A49+1,0)</f>
-        <v>KC_LPRN</v>
+        <v>#N/A</v>
       </c>
       <c r="J49" t="e">
         <f ca="1">VLOOKUP(F49,keys!$A$2:$C$196,$A49+1,0)</f>
@@ -10619,11 +10608,11 @@
       </c>
       <c r="K49" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_v_s_2</v>
+        <v>s_v_2</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, 0, KC_LPRN</v>
+        <v>KC_LPRN, 0</v>
       </c>
       <c r="M49" t="str">
         <f ca="1">VLOOKUP(B49,actions!$A$2:$F$514,5,0)</f>
@@ -10635,7 +10624,7 @@
       </c>
       <c r="O49" t="str">
         <f ca="1">VLOOKUP(B49,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RGUI("`"));</v>
+        <v>SEND_STRING(SS_RCTL("s"));</v>
       </c>
       <c r="P49">
         <f ca="1">VLOOKUP(B49,actions!$A$2:$D$514,4,0)</f>
@@ -10647,19 +10636,19 @@
       </c>
       <c r="R49" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_v_s_2_combo[] = {KC_LPRN, 0, KC_LPRN, COMBO_END};</v>
+        <v>const uint16_t PROGMEM s_v_2_combo[] = {KC_LPRN, 0, COMBO_END};</v>
       </c>
       <c r="S49" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_v_s_2,</v>
+        <v xml:space="preserve">  COMBO_s_v_2,</v>
       </c>
       <c r="T49" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_v_s_2] = COMBO_ACTION(d_v_s_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_s_v_2] = COMBO_ACTION(s_v_2_combo),</v>
       </c>
       <c r="U49" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_d_v_s_2: if (p) {SEND_STRING(SS_RGUI("`"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_s_v_2: if (p) {SEND_STRING(SS_RCTL("s"));}  break;</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -10669,7 +10658,7 @@
       </c>
       <c r="B50" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B50)/2)-1,0)</f>
-        <v>save</v>
+        <v>space</v>
       </c>
       <c r="C50" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C50)/2)-1,0)</f>
@@ -10677,7 +10666,7 @@
       </c>
       <c r="D50" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D50)/2)-1,0)</f>
-        <v>v</v>
+        <v>g</v>
       </c>
       <c r="E50" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E50)/2)-1,0)</f>
@@ -10693,7 +10682,7 @@
       </c>
       <c r="H50" t="str">
         <f ca="1">VLOOKUP(D50,keys!$A$2:$C$196,$A50+1,0)</f>
-        <v>KC_V</v>
+        <v>KC_G</v>
       </c>
       <c r="I50" t="e">
         <f ca="1">VLOOKUP(E50,keys!$A$2:$C$196,$A50+1,0)</f>
@@ -10705,23 +10694,23 @@
       </c>
       <c r="K50" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>s_v_1</v>
+        <v>s_g_1</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_S, KC_V</v>
+        <v>KC_S, KC_G</v>
       </c>
       <c r="M50" t="str">
         <f ca="1">VLOOKUP(B50,actions!$A$2:$F$514,5,0)</f>
-        <v>macro</v>
-      </c>
-      <c r="N50">
+        <v>key</v>
+      </c>
+      <c r="N50" t="str">
         <f ca="1">VLOOKUP(B50,actions!$A$2:$D$514,2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O50" t="str">
+        <v>KC_SPC</v>
+      </c>
+      <c r="O50">
         <f ca="1">VLOOKUP(B50,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("s"));</v>
+        <v>0</v>
       </c>
       <c r="P50">
         <f ca="1">VLOOKUP(B50,actions!$A$2:$D$514,4,0)</f>
@@ -10733,19 +10722,19 @@
       </c>
       <c r="R50" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM s_v_1_combo[] = {KC_S, KC_V, COMBO_END};</v>
+        <v>const uint16_t PROGMEM s_g_1_combo[] = {KC_S, KC_G, COMBO_END};</v>
       </c>
       <c r="S50" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_s_v_1,</v>
+        <v xml:space="preserve">  COMBO_s_g_1,</v>
       </c>
       <c r="T50" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_s_v_1] = COMBO_ACTION(s_v_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_s_g_1] = COMBO(s_g_1_combo, KC_SPC),</v>
       </c>
       <c r="U50" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_s_v_1: if (p) {SEND_STRING(SS_RCTL("s"));}  break;</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -10755,7 +10744,7 @@
       </c>
       <c r="B51" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B51)/2)-1,0)</f>
-        <v>save</v>
+        <v>space</v>
       </c>
       <c r="C51" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C51)/2)-1,0)</f>
@@ -10763,7 +10752,7 @@
       </c>
       <c r="D51" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D51)/2)-1,0)</f>
-        <v>v</v>
+        <v>g</v>
       </c>
       <c r="E51" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E51)/2)-1,0)</f>
@@ -10777,9 +10766,9 @@
         <f ca="1">VLOOKUP(C51,keys!$A$2:$C$196,$A51+1,0)</f>
         <v>KC_LPRN</v>
       </c>
-      <c r="H51">
+      <c r="H51" t="str">
         <f ca="1">VLOOKUP(D51,keys!$A$2:$C$196,$A51+1,0)</f>
-        <v>0</v>
+        <v>KC_TILD</v>
       </c>
       <c r="I51" t="e">
         <f ca="1">VLOOKUP(E51,keys!$A$2:$C$196,$A51+1,0)</f>
@@ -10791,23 +10780,23 @@
       </c>
       <c r="K51" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>s_v_2</v>
+        <v>s_g_2</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, 0</v>
+        <v>KC_LPRN, KC_TILD</v>
       </c>
       <c r="M51" t="str">
         <f ca="1">VLOOKUP(B51,actions!$A$2:$F$514,5,0)</f>
-        <v>macro</v>
-      </c>
-      <c r="N51">
+        <v>key</v>
+      </c>
+      <c r="N51" t="str">
         <f ca="1">VLOOKUP(B51,actions!$A$2:$D$514,2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O51" t="str">
+        <v>KC_SPC</v>
+      </c>
+      <c r="O51">
         <f ca="1">VLOOKUP(B51,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("s"));</v>
+        <v>0</v>
       </c>
       <c r="P51">
         <f ca="1">VLOOKUP(B51,actions!$A$2:$D$514,4,0)</f>
@@ -10815,23 +10804,23 @@
       </c>
       <c r="Q51" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R51" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM s_v_2_combo[] = {KC_LPRN, 0, COMBO_END};</v>
+        <v>const uint16_t PROGMEM s_g_2_combo[] = {KC_LPRN, KC_TILD, COMBO_END};</v>
       </c>
       <c r="S51" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_s_v_2,</v>
+        <v xml:space="preserve">  COMBO_s_g_2,</v>
       </c>
       <c r="T51" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_s_v_2] = COMBO_ACTION(s_v_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_s_g_2] = COMBO(s_g_2_combo, KC_SPC),</v>
       </c>
       <c r="U51" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_s_v_2: if (p) {SEND_STRING(SS_RCTL("s"));}  break;</v>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -10845,7 +10834,7 @@
       </c>
       <c r="C52" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C52)/2)-1,0)</f>
-        <v>s</v>
+        <v>f</v>
       </c>
       <c r="D52" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D52)/2)-1,0)</f>
@@ -10861,7 +10850,7 @@
       </c>
       <c r="G52" t="str">
         <f ca="1">VLOOKUP(C52,keys!$A$2:$C$196,$A52+1,0)</f>
-        <v>KC_S</v>
+        <v>KC_F</v>
       </c>
       <c r="H52" t="str">
         <f ca="1">VLOOKUP(D52,keys!$A$2:$C$196,$A52+1,0)</f>
@@ -10877,11 +10866,11 @@
       </c>
       <c r="K52" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>s_g_1</v>
+        <v>f_g_1</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_S, KC_G</v>
+        <v>KC_F, KC_G</v>
       </c>
       <c r="M52" t="str">
         <f ca="1">VLOOKUP(B52,actions!$A$2:$F$514,5,0)</f>
@@ -10905,15 +10894,15 @@
       </c>
       <c r="R52" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM s_g_1_combo[] = {KC_S, KC_G, COMBO_END};</v>
+        <v>const uint16_t PROGMEM f_g_1_combo[] = {KC_F, KC_G, COMBO_END};</v>
       </c>
       <c r="S52" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_s_g_1,</v>
+        <v xml:space="preserve">  COMBO_f_g_1,</v>
       </c>
       <c r="T52" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_s_g_1] = COMBO(s_g_1_combo, KC_SPC),</v>
+        <v xml:space="preserve">  [COMBO_f_g_1] = COMBO(f_g_1_combo, KC_SPC),</v>
       </c>
       <c r="U52" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -10931,7 +10920,7 @@
       </c>
       <c r="C53" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C53)/2)-1,0)</f>
-        <v>s</v>
+        <v>f</v>
       </c>
       <c r="D53" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D53)/2)-1,0)</f>
@@ -10947,7 +10936,7 @@
       </c>
       <c r="G53" t="str">
         <f ca="1">VLOOKUP(C53,keys!$A$2:$C$196,$A53+1,0)</f>
-        <v>KC_LPRN</v>
+        <v>KC_RPRN</v>
       </c>
       <c r="H53" t="str">
         <f ca="1">VLOOKUP(D53,keys!$A$2:$C$196,$A53+1,0)</f>
@@ -10963,11 +10952,11 @@
       </c>
       <c r="K53" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>s_g_2</v>
+        <v>f_g_2</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, KC_TILD</v>
+        <v>KC_RPRN, KC_TILD</v>
       </c>
       <c r="M53" t="str">
         <f ca="1">VLOOKUP(B53,actions!$A$2:$F$514,5,0)</f>
@@ -10991,15 +10980,15 @@
       </c>
       <c r="R53" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM s_g_2_combo[] = {KC_LPRN, KC_TILD, COMBO_END};</v>
+        <v>const uint16_t PROGMEM f_g_2_combo[] = {KC_RPRN, KC_TILD, COMBO_END};</v>
       </c>
       <c r="S53" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_s_g_2,</v>
+        <v xml:space="preserve">  COMBO_f_g_2,</v>
       </c>
       <c r="T53" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_s_g_2] = COMBO(s_g_2_combo, KC_SPC),</v>
+        <v xml:space="preserve">  [COMBO_f_g_2] = COMBO(f_g_2_combo, KC_SPC),</v>
       </c>
       <c r="U53" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -11013,15 +11002,15 @@
       </c>
       <c r="B54" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B54)/2)-1,0)</f>
-        <v>space</v>
+        <v>tab</v>
       </c>
       <c r="C54" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C54)/2)-1,0)</f>
-        <v>f</v>
+        <v>d</v>
       </c>
       <c r="D54" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D54)/2)-1,0)</f>
-        <v>g</v>
+        <v>f</v>
       </c>
       <c r="E54" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E54)/2)-1,0)</f>
@@ -11033,11 +11022,11 @@
       </c>
       <c r="G54" t="str">
         <f ca="1">VLOOKUP(C54,keys!$A$2:$C$196,$A54+1,0)</f>
-        <v>KC_F</v>
+        <v>KC_D</v>
       </c>
       <c r="H54" t="str">
         <f ca="1">VLOOKUP(D54,keys!$A$2:$C$196,$A54+1,0)</f>
-        <v>KC_G</v>
+        <v>KC_F</v>
       </c>
       <c r="I54" t="e">
         <f ca="1">VLOOKUP(E54,keys!$A$2:$C$196,$A54+1,0)</f>
@@ -11049,11 +11038,11 @@
       </c>
       <c r="K54" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>f_g_1</v>
+        <v>d_f_1</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_F, KC_G</v>
+        <v>KC_D, KC_F</v>
       </c>
       <c r="M54" t="str">
         <f ca="1">VLOOKUP(B54,actions!$A$2:$F$514,5,0)</f>
@@ -11061,7 +11050,7 @@
       </c>
       <c r="N54" t="str">
         <f ca="1">VLOOKUP(B54,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_SPC</v>
+        <v>KC_TAB</v>
       </c>
       <c r="O54">
         <f ca="1">VLOOKUP(B54,actions!$A$2:$D$514,3,0)</f>
@@ -11077,15 +11066,15 @@
       </c>
       <c r="R54" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM f_g_1_combo[] = {KC_F, KC_G, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_f_1_combo[] = {KC_D, KC_F, COMBO_END};</v>
       </c>
       <c r="S54" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_f_g_1,</v>
+        <v xml:space="preserve">  COMBO_d_f_1,</v>
       </c>
       <c r="T54" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_f_g_1] = COMBO(f_g_1_combo, KC_SPC),</v>
+        <v xml:space="preserve">  [COMBO_d_f_1] = COMBO(d_f_1_combo, KC_TAB),</v>
       </c>
       <c r="U54" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -11099,15 +11088,15 @@
       </c>
       <c r="B55" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B55)/2)-1,0)</f>
-        <v>space</v>
+        <v>tab</v>
       </c>
       <c r="C55" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C55)/2)-1,0)</f>
-        <v>f</v>
+        <v>d</v>
       </c>
       <c r="D55" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D55)/2)-1,0)</f>
-        <v>g</v>
+        <v>f</v>
       </c>
       <c r="E55" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E55)/2)-1,0)</f>
@@ -11119,11 +11108,11 @@
       </c>
       <c r="G55" t="str">
         <f ca="1">VLOOKUP(C55,keys!$A$2:$C$196,$A55+1,0)</f>
-        <v>KC_RPRN</v>
+        <v>KC_LPRN</v>
       </c>
       <c r="H55" t="str">
         <f ca="1">VLOOKUP(D55,keys!$A$2:$C$196,$A55+1,0)</f>
-        <v>KC_TILD</v>
+        <v>KC_RPRN</v>
       </c>
       <c r="I55" t="e">
         <f ca="1">VLOOKUP(E55,keys!$A$2:$C$196,$A55+1,0)</f>
@@ -11135,11 +11124,11 @@
       </c>
       <c r="K55" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>f_g_2</v>
+        <v>d_f_2</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_RPRN, KC_TILD</v>
+        <v>KC_LPRN, KC_RPRN</v>
       </c>
       <c r="M55" t="str">
         <f ca="1">VLOOKUP(B55,actions!$A$2:$F$514,5,0)</f>
@@ -11147,7 +11136,7 @@
       </c>
       <c r="N55" t="str">
         <f ca="1">VLOOKUP(B55,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_SPC</v>
+        <v>KC_TAB</v>
       </c>
       <c r="O55">
         <f ca="1">VLOOKUP(B55,actions!$A$2:$D$514,3,0)</f>
@@ -11163,15 +11152,15 @@
       </c>
       <c r="R55" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM f_g_2_combo[] = {KC_RPRN, KC_TILD, COMBO_END};</v>
+        <v>const uint16_t PROGMEM d_f_2_combo[] = {KC_LPRN, KC_RPRN, COMBO_END};</v>
       </c>
       <c r="S55" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_f_g_2,</v>
+        <v xml:space="preserve">  COMBO_d_f_2,</v>
       </c>
       <c r="T55" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_f_g_2] = COMBO(f_g_2_combo, KC_SPC),</v>
+        <v xml:space="preserve">  [COMBO_d_f_2] = COMBO(d_f_2_combo, KC_TAB),</v>
       </c>
       <c r="U55" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -11185,15 +11174,15 @@
       </c>
       <c r="B56" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B56)/2)-1,0)</f>
-        <v>tab</v>
+        <v>undo</v>
       </c>
       <c r="C56" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C56)/2)-1,0)</f>
-        <v>d</v>
+        <v>z</v>
       </c>
       <c r="D56" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D56)/2)-1,0)</f>
-        <v>f</v>
+        <v>s</v>
       </c>
       <c r="E56" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E56)/2)-1,0)</f>
@@ -11205,11 +11194,11 @@
       </c>
       <c r="G56" t="str">
         <f ca="1">VLOOKUP(C56,keys!$A$2:$C$196,$A56+1,0)</f>
-        <v>KC_D</v>
+        <v>KC_Z</v>
       </c>
       <c r="H56" t="str">
         <f ca="1">VLOOKUP(D56,keys!$A$2:$C$196,$A56+1,0)</f>
-        <v>KC_F</v>
+        <v>KC_S</v>
       </c>
       <c r="I56" t="e">
         <f ca="1">VLOOKUP(E56,keys!$A$2:$C$196,$A56+1,0)</f>
@@ -11221,23 +11210,23 @@
       </c>
       <c r="K56" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_f_1</v>
+        <v>z_s_1</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_D, KC_F</v>
+        <v>KC_Z, KC_S</v>
       </c>
       <c r="M56" t="str">
         <f ca="1">VLOOKUP(B56,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N56" t="str">
+        <v>macro</v>
+      </c>
+      <c r="N56">
         <f ca="1">VLOOKUP(B56,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_TAB</v>
-      </c>
-      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="O56" t="str">
         <f ca="1">VLOOKUP(B56,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
+        <v>SEND_STRING(SS_RCTL("z"));</v>
       </c>
       <c r="P56">
         <f ca="1">VLOOKUP(B56,actions!$A$2:$D$514,4,0)</f>
@@ -11249,19 +11238,19 @@
       </c>
       <c r="R56" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_f_1_combo[] = {KC_D, KC_F, COMBO_END};</v>
+        <v>const uint16_t PROGMEM z_s_1_combo[] = {KC_Z, KC_S, COMBO_END};</v>
       </c>
       <c r="S56" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_f_1,</v>
+        <v xml:space="preserve">  COMBO_z_s_1,</v>
       </c>
       <c r="T56" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_f_1] = COMBO(d_f_1_combo, KC_TAB),</v>
+        <v xml:space="preserve">  [COMBO_z_s_1] = COMBO_ACTION(z_s_1_combo),</v>
       </c>
       <c r="U56" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v xml:space="preserve">    case COMBO_z_s_1: if (p) {SEND_STRING(SS_RCTL("z"));}  break;</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -11271,15 +11260,15 @@
       </c>
       <c r="B57" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B57)/2)-1,0)</f>
-        <v>tab</v>
+        <v>undo</v>
       </c>
       <c r="C57" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C57)/2)-1,0)</f>
-        <v>d</v>
+        <v>z</v>
       </c>
       <c r="D57" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D57)/2)-1,0)</f>
-        <v>f</v>
+        <v>s</v>
       </c>
       <c r="E57" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E57)/2)-1,0)</f>
@@ -11289,13 +11278,13 @@
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F57)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G57" t="str">
+      <c r="G57">
         <f ca="1">VLOOKUP(C57,keys!$A$2:$C$196,$A57+1,0)</f>
-        <v>KC_LPRN</v>
+        <v>0</v>
       </c>
       <c r="H57" t="str">
         <f ca="1">VLOOKUP(D57,keys!$A$2:$C$196,$A57+1,0)</f>
-        <v>KC_RPRN</v>
+        <v>KC_LPRN</v>
       </c>
       <c r="I57" t="e">
         <f ca="1">VLOOKUP(E57,keys!$A$2:$C$196,$A57+1,0)</f>
@@ -11307,23 +11296,23 @@
       </c>
       <c r="K57" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>d_f_2</v>
+        <v>z_s_2</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_LPRN, KC_RPRN</v>
+        <v>0, KC_LPRN</v>
       </c>
       <c r="M57" t="str">
         <f ca="1">VLOOKUP(B57,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N57" t="str">
+        <v>macro</v>
+      </c>
+      <c r="N57">
         <f ca="1">VLOOKUP(B57,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_TAB</v>
-      </c>
-      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="O57" t="str">
         <f ca="1">VLOOKUP(B57,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
+        <v>SEND_STRING(SS_RCTL("z"));</v>
       </c>
       <c r="P57">
         <f ca="1">VLOOKUP(B57,actions!$A$2:$D$514,4,0)</f>
@@ -11331,23 +11320,23 @@
       </c>
       <c r="Q57" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM d_f_2_combo[] = {KC_LPRN, KC_RPRN, COMBO_END};</v>
+        <v>const uint16_t PROGMEM z_s_2_combo[] = {0, KC_LPRN, COMBO_END};</v>
       </c>
       <c r="S57" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_d_f_2,</v>
+        <v xml:space="preserve">  COMBO_z_s_2,</v>
       </c>
       <c r="T57" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_d_f_2] = COMBO(d_f_2_combo, KC_TAB),</v>
+        <v xml:space="preserve">  [COMBO_z_s_2] = COMBO_ACTION(z_s_2_combo),</v>
       </c>
       <c r="U57" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v xml:space="preserve">    case COMBO_z_s_2: if (p) {SEND_STRING(SS_RCTL("z"));}  break;</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -11357,15 +11346,15 @@
       </c>
       <c r="B58" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B58)/2)-1,0)</f>
-        <v>undo</v>
+        <v>word_left</v>
       </c>
       <c r="C58" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C58)/2)-1,0)</f>
-        <v>z</v>
+        <v>m</v>
       </c>
       <c r="D58" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D58)/2)-1,0)</f>
-        <v>s</v>
+        <v>coma</v>
       </c>
       <c r="E58" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E58)/2)-1,0)</f>
@@ -11377,11 +11366,11 @@
       </c>
       <c r="G58" t="str">
         <f ca="1">VLOOKUP(C58,keys!$A$2:$C$196,$A58+1,0)</f>
-        <v>KC_Z</v>
+        <v>KC_M</v>
       </c>
       <c r="H58" t="str">
         <f ca="1">VLOOKUP(D58,keys!$A$2:$C$196,$A58+1,0)</f>
-        <v>KC_S</v>
+        <v>KC_COMM</v>
       </c>
       <c r="I58" t="e">
         <f ca="1">VLOOKUP(E58,keys!$A$2:$C$196,$A58+1,0)</f>
@@ -11393,11 +11382,11 @@
       </c>
       <c r="K58" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>z_s_1</v>
+        <v>m_coma_1</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_Z, KC_S</v>
+        <v>KC_M, KC_COMM</v>
       </c>
       <c r="M58" t="str">
         <f ca="1">VLOOKUP(B58,actions!$A$2:$F$514,5,0)</f>
@@ -11409,11 +11398,11 @@
       </c>
       <c r="O58" t="str">
         <f ca="1">VLOOKUP(B58,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("z"));</v>
-      </c>
-      <c r="P58">
+        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));</v>
+      </c>
+      <c r="P58" t="str">
         <f ca="1">VLOOKUP(B58,actions!$A$2:$D$514,4,0)</f>
-        <v>0</v>
+        <v>SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));</v>
       </c>
       <c r="Q58" t="b">
         <f t="shared" ca="1" si="3"/>
@@ -11421,19 +11410,19 @@
       </c>
       <c r="R58" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM z_s_1_combo[] = {KC_Z, KC_S, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_coma_1_combo[] = {KC_M, KC_COMM, COMBO_END};</v>
       </c>
       <c r="S58" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_z_s_1,</v>
+        <v xml:space="preserve">  COMBO_m_coma_1,</v>
       </c>
       <c r="T58" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_z_s_1] = COMBO_ACTION(z_s_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_m_coma_1] = COMBO_ACTION(m_coma_1_combo),</v>
       </c>
       <c r="U58" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_z_s_1: if (p) {SEND_STRING(SS_RCTL("z"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_m_coma_1: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));} else {SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));} break;</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -11443,15 +11432,15 @@
       </c>
       <c r="B59" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B59)/2)-1,0)</f>
-        <v>undo</v>
+        <v>word_left</v>
       </c>
       <c r="C59" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C59)/2)-1,0)</f>
-        <v>z</v>
+        <v>m</v>
       </c>
       <c r="D59" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D59)/2)-1,0)</f>
-        <v>s</v>
+        <v>coma</v>
       </c>
       <c r="E59" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E59)/2)-1,0)</f>
@@ -11461,13 +11450,13 @@
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F59)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G59">
+      <c r="G59" t="str">
         <f ca="1">VLOOKUP(C59,keys!$A$2:$C$196,$A59+1,0)</f>
-        <v>0</v>
+        <v>KC_1</v>
       </c>
       <c r="H59" t="str">
         <f ca="1">VLOOKUP(D59,keys!$A$2:$C$196,$A59+1,0)</f>
-        <v>KC_LPRN</v>
+        <v>KC_2</v>
       </c>
       <c r="I59" t="e">
         <f ca="1">VLOOKUP(E59,keys!$A$2:$C$196,$A59+1,0)</f>
@@ -11479,11 +11468,11 @@
       </c>
       <c r="K59" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>z_s_2</v>
+        <v>m_coma_2</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0, KC_LPRN</v>
+        <v>KC_1, KC_2</v>
       </c>
       <c r="M59" t="str">
         <f ca="1">VLOOKUP(B59,actions!$A$2:$F$514,5,0)</f>
@@ -11495,31 +11484,31 @@
       </c>
       <c r="O59" t="str">
         <f ca="1">VLOOKUP(B59,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_RCTL("z"));</v>
-      </c>
-      <c r="P59">
+        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));</v>
+      </c>
+      <c r="P59" t="str">
         <f ca="1">VLOOKUP(B59,actions!$A$2:$D$514,4,0)</f>
-        <v>0</v>
+        <v>SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));</v>
       </c>
       <c r="Q59" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM z_s_2_combo[] = {0, KC_LPRN, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_coma_2_combo[] = {KC_1, KC_2, COMBO_END};</v>
       </c>
       <c r="S59" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_z_s_2,</v>
+        <v xml:space="preserve">  COMBO_m_coma_2,</v>
       </c>
       <c r="T59" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_z_s_2] = COMBO_ACTION(z_s_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_m_coma_2] = COMBO_ACTION(m_coma_2_combo),</v>
       </c>
       <c r="U59" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_z_s_2: if (p) {SEND_STRING(SS_RCTL("z"));}  break;</v>
+        <v xml:space="preserve">    case COMBO_m_coma_2: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));} else {SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));} break;</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -11529,15 +11518,15 @@
       </c>
       <c r="B60" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B60)/2)-1,0)</f>
-        <v>word_left</v>
+        <v>word_right</v>
       </c>
       <c r="C60" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C60)/2)-1,0)</f>
-        <v>m</v>
+        <v>coma</v>
       </c>
       <c r="D60" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D60)/2)-1,0)</f>
-        <v>coma</v>
+        <v>dot</v>
       </c>
       <c r="E60" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E60)/2)-1,0)</f>
@@ -11549,11 +11538,11 @@
       </c>
       <c r="G60" t="str">
         <f ca="1">VLOOKUP(C60,keys!$A$2:$C$196,$A60+1,0)</f>
-        <v>KC_M</v>
+        <v>KC_COMM</v>
       </c>
       <c r="H60" t="str">
         <f ca="1">VLOOKUP(D60,keys!$A$2:$C$196,$A60+1,0)</f>
-        <v>KC_COMM</v>
+        <v>KC_DOT</v>
       </c>
       <c r="I60" t="e">
         <f ca="1">VLOOKUP(E60,keys!$A$2:$C$196,$A60+1,0)</f>
@@ -11565,11 +11554,11 @@
       </c>
       <c r="K60" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_coma_1</v>
+        <v>coma_dot_1</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_M, KC_COMM</v>
+        <v>KC_COMM, KC_DOT</v>
       </c>
       <c r="M60" t="str">
         <f ca="1">VLOOKUP(B60,actions!$A$2:$F$514,5,0)</f>
@@ -11581,11 +11570,11 @@
       </c>
       <c r="O60" t="str">
         <f ca="1">VLOOKUP(B60,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));</v>
+        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));</v>
       </c>
       <c r="P60" t="str">
         <f ca="1">VLOOKUP(B60,actions!$A$2:$D$514,4,0)</f>
-        <v>SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));</v>
+        <v>SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));</v>
       </c>
       <c r="Q60" t="b">
         <f t="shared" ca="1" si="3"/>
@@ -11593,19 +11582,19 @@
       </c>
       <c r="R60" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_coma_1_combo[] = {KC_M, KC_COMM, COMBO_END};</v>
+        <v>const uint16_t PROGMEM coma_dot_1_combo[] = {KC_COMM, KC_DOT, COMBO_END};</v>
       </c>
       <c r="S60" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_coma_1,</v>
+        <v xml:space="preserve">  COMBO_coma_dot_1,</v>
       </c>
       <c r="T60" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_coma_1] = COMBO_ACTION(m_coma_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_coma_dot_1] = COMBO_ACTION(coma_dot_1_combo),</v>
       </c>
       <c r="U60" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_m_coma_1: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));} else {SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));} break;</v>
+        <v xml:space="preserve">    case COMBO_coma_dot_1: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));} else {SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));} break;</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -11615,15 +11604,15 @@
       </c>
       <c r="B61" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B61)/2)-1,0)</f>
-        <v>word_left</v>
+        <v>word_right</v>
       </c>
       <c r="C61" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C61)/2)-1,0)</f>
-        <v>m</v>
+        <v>coma</v>
       </c>
       <c r="D61" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D61)/2)-1,0)</f>
-        <v>coma</v>
+        <v>dot</v>
       </c>
       <c r="E61" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E61)/2)-1,0)</f>
@@ -11635,11 +11624,11 @@
       </c>
       <c r="G61" t="str">
         <f ca="1">VLOOKUP(C61,keys!$A$2:$C$196,$A61+1,0)</f>
-        <v>KC_1</v>
+        <v>KC_2</v>
       </c>
       <c r="H61" t="str">
         <f ca="1">VLOOKUP(D61,keys!$A$2:$C$196,$A61+1,0)</f>
-        <v>KC_2</v>
+        <v>KC_3</v>
       </c>
       <c r="I61" t="e">
         <f ca="1">VLOOKUP(E61,keys!$A$2:$C$196,$A61+1,0)</f>
@@ -11651,11 +11640,11 @@
       </c>
       <c r="K61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_coma_2</v>
+        <v>coma_dot_2</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_1, KC_2</v>
+        <v>KC_2, KC_3</v>
       </c>
       <c r="M61" t="str">
         <f ca="1">VLOOKUP(B61,actions!$A$2:$F$514,5,0)</f>
@@ -11667,11 +11656,11 @@
       </c>
       <c r="O61" t="str">
         <f ca="1">VLOOKUP(B61,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));</v>
+        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));</v>
       </c>
       <c r="P61" t="str">
         <f ca="1">VLOOKUP(B61,actions!$A$2:$D$514,4,0)</f>
-        <v>SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));</v>
+        <v>SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));</v>
       </c>
       <c r="Q61" t="b">
         <f t="shared" ca="1" si="3"/>
@@ -11679,19 +11668,19 @@
       </c>
       <c r="R61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_coma_2_combo[] = {KC_1, KC_2, COMBO_END};</v>
+        <v>const uint16_t PROGMEM coma_dot_2_combo[] = {KC_2, KC_3, COMBO_END};</v>
       </c>
       <c r="S61" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_coma_2,</v>
+        <v xml:space="preserve">  COMBO_coma_dot_2,</v>
       </c>
       <c r="T61" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_coma_2] = COMBO_ACTION(m_coma_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_coma_dot_2] = COMBO_ACTION(coma_dot_2_combo),</v>
       </c>
       <c r="U61" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_m_coma_2: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_LEFT));} else {SEND_STRING(SS_UP(X_LEFT)SS_UP(X_RCTL));} break;</v>
+        <v xml:space="preserve">    case COMBO_coma_dot_2: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));} else {SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));} break;</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -11701,15 +11690,15 @@
       </c>
       <c r="B62" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B62)/2)-1,0)</f>
-        <v>word_right</v>
+        <v>left</v>
       </c>
       <c r="C62" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C62)/2)-1,0)</f>
-        <v>coma</v>
+        <v>m</v>
       </c>
       <c r="D62" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D62)/2)-1,0)</f>
-        <v>dot</v>
+        <v>k</v>
       </c>
       <c r="E62" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E62)/2)-1,0)</f>
@@ -11721,11 +11710,11 @@
       </c>
       <c r="G62" t="str">
         <f ca="1">VLOOKUP(C62,keys!$A$2:$C$196,$A62+1,0)</f>
-        <v>KC_COMM</v>
+        <v>KC_M</v>
       </c>
       <c r="H62" t="str">
         <f ca="1">VLOOKUP(D62,keys!$A$2:$C$196,$A62+1,0)</f>
-        <v>KC_DOT</v>
+        <v>KC_K</v>
       </c>
       <c r="I62" t="e">
         <f ca="1">VLOOKUP(E62,keys!$A$2:$C$196,$A62+1,0)</f>
@@ -11737,27 +11726,27 @@
       </c>
       <c r="K62" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>coma_dot_1</v>
+        <v>m_k_1</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_COMM, KC_DOT</v>
+        <v>KC_M, KC_K</v>
       </c>
       <c r="M62" t="str">
         <f ca="1">VLOOKUP(B62,actions!$A$2:$F$514,5,0)</f>
-        <v>macro</v>
-      </c>
-      <c r="N62">
+        <v>key</v>
+      </c>
+      <c r="N62" t="str">
         <f ca="1">VLOOKUP(B62,actions!$A$2:$D$514,2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O62" t="str">
+        <v>KC_LEFT</v>
+      </c>
+      <c r="O62">
         <f ca="1">VLOOKUP(B62,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));</v>
-      </c>
-      <c r="P62" t="str">
+        <v>0</v>
+      </c>
+      <c r="P62">
         <f ca="1">VLOOKUP(B62,actions!$A$2:$D$514,4,0)</f>
-        <v>SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));</v>
+        <v>0</v>
       </c>
       <c r="Q62" t="b">
         <f t="shared" ca="1" si="3"/>
@@ -11765,19 +11754,19 @@
       </c>
       <c r="R62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM coma_dot_1_combo[] = {KC_COMM, KC_DOT, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_k_1_combo[] = {KC_M, KC_K, COMBO_END};</v>
       </c>
       <c r="S62" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_coma_dot_1,</v>
+        <v xml:space="preserve">  COMBO_m_k_1,</v>
       </c>
       <c r="T62" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_coma_dot_1] = COMBO_ACTION(coma_dot_1_combo),</v>
+        <v xml:space="preserve">  [COMBO_m_k_1] = COMBO(m_k_1_combo, KC_LEFT),</v>
       </c>
       <c r="U62" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_coma_dot_1: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));} else {SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));} break;</v>
+        <v/>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -11787,15 +11776,15 @@
       </c>
       <c r="B63" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B63)/2)-1,0)</f>
-        <v>word_right</v>
+        <v>left</v>
       </c>
       <c r="C63" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C63)/2)-1,0)</f>
-        <v>coma</v>
+        <v>m</v>
       </c>
       <c r="D63" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D63)/2)-1,0)</f>
-        <v>dot</v>
+        <v>k</v>
       </c>
       <c r="E63" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E63)/2)-1,0)</f>
@@ -11807,11 +11796,11 @@
       </c>
       <c r="G63" t="str">
         <f ca="1">VLOOKUP(C63,keys!$A$2:$C$196,$A63+1,0)</f>
-        <v>KC_2</v>
+        <v>KC_1</v>
       </c>
       <c r="H63" t="str">
         <f ca="1">VLOOKUP(D63,keys!$A$2:$C$196,$A63+1,0)</f>
-        <v>KC_3</v>
+        <v>KC_5</v>
       </c>
       <c r="I63" t="e">
         <f ca="1">VLOOKUP(E63,keys!$A$2:$C$196,$A63+1,0)</f>
@@ -11823,27 +11812,27 @@
       </c>
       <c r="K63" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>coma_dot_2</v>
+        <v>m_k_2</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_2, KC_3</v>
+        <v>KC_1, KC_5</v>
       </c>
       <c r="M63" t="str">
         <f ca="1">VLOOKUP(B63,actions!$A$2:$F$514,5,0)</f>
-        <v>macro</v>
-      </c>
-      <c r="N63">
+        <v>key</v>
+      </c>
+      <c r="N63" t="str">
         <f ca="1">VLOOKUP(B63,actions!$A$2:$D$514,2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O63" t="str">
+        <v>KC_LEFT</v>
+      </c>
+      <c r="O63">
         <f ca="1">VLOOKUP(B63,actions!$A$2:$D$514,3,0)</f>
-        <v>SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));</v>
-      </c>
-      <c r="P63" t="str">
+        <v>0</v>
+      </c>
+      <c r="P63">
         <f ca="1">VLOOKUP(B63,actions!$A$2:$D$514,4,0)</f>
-        <v>SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));</v>
+        <v>0</v>
       </c>
       <c r="Q63" t="b">
         <f t="shared" ca="1" si="3"/>
@@ -11851,19 +11840,19 @@
       </c>
       <c r="R63" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM coma_dot_2_combo[] = {KC_2, KC_3, COMBO_END};</v>
+        <v>const uint16_t PROGMEM m_k_2_combo[] = {KC_1, KC_5, COMBO_END};</v>
       </c>
       <c r="S63" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_coma_dot_2,</v>
+        <v xml:space="preserve">  COMBO_m_k_2,</v>
       </c>
       <c r="T63" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_coma_dot_2] = COMBO_ACTION(coma_dot_2_combo),</v>
+        <v xml:space="preserve">  [COMBO_m_k_2] = COMBO(m_k_2_combo, KC_LEFT),</v>
       </c>
       <c r="U63" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    case COMBO_coma_dot_2: if (p) {SEND_STRING(SS_DOWN(X_RCTL)SS_DOWN(X_RGHT));} else {SEND_STRING(SS_UP(X_RGHT)SS_UP(X_RCTL));} break;</v>
+        <v/>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -11873,15 +11862,15 @@
       </c>
       <c r="B64" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B64)/2)-1,0)</f>
-        <v>left</v>
+        <v>right</v>
       </c>
       <c r="C64" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C64)/2)-1,0)</f>
-        <v>m</v>
+        <v>k</v>
       </c>
       <c r="D64" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D64)/2)-1,0)</f>
-        <v>k</v>
+        <v>dot</v>
       </c>
       <c r="E64" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E64)/2)-1,0)</f>
@@ -11893,11 +11882,11 @@
       </c>
       <c r="G64" t="str">
         <f ca="1">VLOOKUP(C64,keys!$A$2:$C$196,$A64+1,0)</f>
-        <v>KC_M</v>
+        <v>KC_K</v>
       </c>
       <c r="H64" t="str">
         <f ca="1">VLOOKUP(D64,keys!$A$2:$C$196,$A64+1,0)</f>
-        <v>KC_K</v>
+        <v>KC_DOT</v>
       </c>
       <c r="I64" t="e">
         <f ca="1">VLOOKUP(E64,keys!$A$2:$C$196,$A64+1,0)</f>
@@ -11909,11 +11898,11 @@
       </c>
       <c r="K64" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_k_1</v>
+        <v>k_dot_1</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_M, KC_K</v>
+        <v>KC_K, KC_DOT</v>
       </c>
       <c r="M64" t="str">
         <f ca="1">VLOOKUP(B64,actions!$A$2:$F$514,5,0)</f>
@@ -11921,7 +11910,7 @@
       </c>
       <c r="N64" t="str">
         <f ca="1">VLOOKUP(B64,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_LEFT</v>
+        <v>KC_RGHT</v>
       </c>
       <c r="O64">
         <f ca="1">VLOOKUP(B64,actions!$A$2:$D$514,3,0)</f>
@@ -11937,15 +11926,15 @@
       </c>
       <c r="R64" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_k_1_combo[] = {KC_M, KC_K, COMBO_END};</v>
+        <v>const uint16_t PROGMEM k_dot_1_combo[] = {KC_K, KC_DOT, COMBO_END};</v>
       </c>
       <c r="S64" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_k_1,</v>
+        <v xml:space="preserve">  COMBO_k_dot_1,</v>
       </c>
       <c r="T64" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_k_1] = COMBO(m_k_1_combo, KC_LEFT),</v>
+        <v xml:space="preserve">  [COMBO_k_dot_1] = COMBO(k_dot_1_combo, KC_RGHT),</v>
       </c>
       <c r="U64" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -11959,15 +11948,15 @@
       </c>
       <c r="B65" t="str">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B65)/2)-1,0)</f>
-        <v>left</v>
+        <v>right</v>
       </c>
       <c r="C65" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C65)/2)-1,0)</f>
-        <v>m</v>
+        <v>k</v>
       </c>
       <c r="D65" s="3" t="str">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D65)/2)-1,0)</f>
-        <v>k</v>
+        <v>dot</v>
       </c>
       <c r="E65" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E65)/2)-1,0)</f>
@@ -11979,11 +11968,11 @@
       </c>
       <c r="G65" t="str">
         <f ca="1">VLOOKUP(C65,keys!$A$2:$C$196,$A65+1,0)</f>
-        <v>KC_1</v>
+        <v>KC_5</v>
       </c>
       <c r="H65" t="str">
         <f ca="1">VLOOKUP(D65,keys!$A$2:$C$196,$A65+1,0)</f>
-        <v>KC_5</v>
+        <v>KC_3</v>
       </c>
       <c r="I65" t="e">
         <f ca="1">VLOOKUP(E65,keys!$A$2:$C$196,$A65+1,0)</f>
@@ -11995,11 +11984,11 @@
       </c>
       <c r="K65" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>m_k_2</v>
+        <v>k_dot_2</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KC_1, KC_5</v>
+        <v>KC_5, KC_3</v>
       </c>
       <c r="M65" t="str">
         <f ca="1">VLOOKUP(B65,actions!$A$2:$F$514,5,0)</f>
@@ -12007,7 +11996,7 @@
       </c>
       <c r="N65" t="str">
         <f ca="1">VLOOKUP(B65,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_LEFT</v>
+        <v>KC_RGHT</v>
       </c>
       <c r="O65">
         <f ca="1">VLOOKUP(B65,actions!$A$2:$D$514,3,0)</f>
@@ -12023,15 +12012,15 @@
       </c>
       <c r="R65" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>const uint16_t PROGMEM m_k_2_combo[] = {KC_1, KC_5, COMBO_END};</v>
+        <v>const uint16_t PROGMEM k_dot_2_combo[] = {KC_5, KC_3, COMBO_END};</v>
       </c>
       <c r="S65" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v xml:space="preserve">  COMBO_m_k_2,</v>
+        <v xml:space="preserve">  COMBO_k_dot_2,</v>
       </c>
       <c r="T65" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">  [COMBO_m_k_2] = COMBO(m_k_2_combo, KC_LEFT),</v>
+        <v xml:space="preserve">  [COMBO_k_dot_2] = COMBO(k_dot_2_combo, KC_RGHT),</v>
       </c>
       <c r="U65" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -12043,17 +12032,17 @@
         <f t="shared" ref="A66:A129" si="9">MOD(ROW(A66),2)+1</f>
         <v>1</v>
       </c>
-      <c r="B66" t="str">
+      <c r="B66">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B66)/2)-1,0)</f>
-        <v>right</v>
-      </c>
-      <c r="C66" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C66)/2)-1,0)</f>
-        <v>k</v>
-      </c>
-      <c r="D66" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D66)/2)-1,0)</f>
-        <v>dot</v>
+        <v>0</v>
       </c>
       <c r="E66" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E66)/2)-1,0)</f>
@@ -12063,13 +12052,13 @@
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F66)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G66" t="str">
+      <c r="G66" t="e">
         <f ca="1">VLOOKUP(C66,keys!$A$2:$C$196,$A66+1,0)</f>
-        <v>KC_K</v>
-      </c>
-      <c r="H66" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="H66" t="e">
         <f ca="1">VLOOKUP(D66,keys!$A$2:$C$196,$A66+1,0)</f>
-        <v>KC_DOT</v>
+        <v>#N/A</v>
       </c>
       <c r="I66" t="e">
         <f ca="1">VLOOKUP(E66,keys!$A$2:$C$196,$A66+1,0)</f>
@@ -12081,47 +12070,47 @@
       </c>
       <c r="K66" t="str">
         <f t="shared" ref="K66:K129" ca="1" si="10">C66&amp;"_"&amp;D66&amp;IF(ISNA(I66),"","_"&amp;E66&amp;IF(ISNA(J66),"","_"&amp;F66))&amp;"_"&amp;TEXT(A66,"0")</f>
-        <v>k_dot_1</v>
-      </c>
-      <c r="L66" t="str">
+        <v>0_0_1</v>
+      </c>
+      <c r="L66" t="e">
         <f t="shared" ref="L66:L129" ca="1" si="11">G66&amp;", "&amp;H66&amp;IF(ISNA(I66),"",", "&amp;I66&amp;IF(ISNA(J66),"",", "&amp;J66))</f>
-        <v>KC_K, KC_DOT</v>
-      </c>
-      <c r="M66" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M66" t="e">
         <f ca="1">VLOOKUP(B66,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N66" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N66" t="e">
         <f ca="1">VLOOKUP(B66,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_RGHT</v>
-      </c>
-      <c r="O66">
+        <v>#N/A</v>
+      </c>
+      <c r="O66" t="e">
         <f ca="1">VLOOKUP(B66,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P66">
+        <v>#N/A</v>
+      </c>
+      <c r="P66" t="e">
         <f ca="1">VLOOKUP(B66,actions!$A$2:$D$514,4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q66" t="b">
+        <v>#N/A</v>
+      </c>
+      <c r="Q66" t="e">
         <f t="shared" ref="Q66:Q129" ca="1" si="12">AND(B66&lt;&gt;0,G66&lt;&gt;0,H66&lt;&gt;0)</f>
-        <v>1</v>
-      </c>
-      <c r="R66" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R66" t="e">
         <f t="shared" ref="R66:R129" ca="1" si="13">"const uint16_t PROGMEM "&amp;K66&amp;"_combo[] = {"&amp;L66&amp;", COMBO_END};"</f>
-        <v>const uint16_t PROGMEM k_dot_1_combo[] = {KC_K, KC_DOT, COMBO_END};</v>
+        <v>#N/A</v>
       </c>
       <c r="S66" t="str">
         <f t="shared" ref="S66:S129" ca="1" si="14">"  COMBO_"&amp;K66&amp;","</f>
-        <v xml:space="preserve">  COMBO_k_dot_1,</v>
-      </c>
-      <c r="T66" t="str">
+        <v xml:space="preserve">  COMBO_0_0_1,</v>
+      </c>
+      <c r="T66" t="e">
         <f t="shared" ref="T66:T129" ca="1" si="15">"  [COMBO_"&amp;K66&amp;"] = COMBO"&amp;IF(M66="key","","_ACTION")&amp;"("&amp;K66&amp;"_combo"&amp;IF(M66="key",", "&amp;N66,"")&amp;"),"</f>
-        <v xml:space="preserve">  [COMBO_k_dot_1] = COMBO(k_dot_1_combo, KC_RGHT),</v>
-      </c>
-      <c r="U66" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U66" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -12129,17 +12118,17 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="B67" t="str">
+      <c r="B67">
         <f ca="1">OFFSET(actions_combos!A$2,_xlfn.FLOOR.MATH(ROW(B67)/2)-1,0)</f>
-        <v>right</v>
-      </c>
-      <c r="C67" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3">
         <f ca="1">OFFSET(actions_combos!B$2,_xlfn.FLOOR.MATH(ROW(C67)/2)-1,0)</f>
-        <v>k</v>
-      </c>
-      <c r="D67" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3">
         <f ca="1">OFFSET(actions_combos!C$2,_xlfn.FLOOR.MATH(ROW(D67)/2)-1,0)</f>
-        <v>dot</v>
+        <v>0</v>
       </c>
       <c r="E67" s="3">
         <f ca="1">OFFSET(actions_combos!D$2,_xlfn.FLOOR.MATH(ROW(E67)/2)-1,0)</f>
@@ -12149,13 +12138,13 @@
         <f ca="1">OFFSET(actions_combos!E$2,_xlfn.FLOOR.MATH(ROW(F67)/2)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="G67" t="str">
+      <c r="G67" t="e">
         <f ca="1">VLOOKUP(C67,keys!$A$2:$C$196,$A67+1,0)</f>
-        <v>KC_5</v>
-      </c>
-      <c r="H67" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="H67" t="e">
         <f ca="1">VLOOKUP(D67,keys!$A$2:$C$196,$A67+1,0)</f>
-        <v>KC_3</v>
+        <v>#N/A</v>
       </c>
       <c r="I67" t="e">
         <f ca="1">VLOOKUP(E67,keys!$A$2:$C$196,$A67+1,0)</f>
@@ -12167,47 +12156,47 @@
       </c>
       <c r="K67" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>k_dot_2</v>
-      </c>
-      <c r="L67" t="str">
+        <v>0_0_2</v>
+      </c>
+      <c r="L67" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>KC_5, KC_3</v>
-      </c>
-      <c r="M67" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M67" t="e">
         <f ca="1">VLOOKUP(B67,actions!$A$2:$F$514,5,0)</f>
-        <v>key</v>
-      </c>
-      <c r="N67" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N67" t="e">
         <f ca="1">VLOOKUP(B67,actions!$A$2:$D$514,2,0)</f>
-        <v>KC_RGHT</v>
-      </c>
-      <c r="O67">
+        <v>#N/A</v>
+      </c>
+      <c r="O67" t="e">
         <f ca="1">VLOOKUP(B67,actions!$A$2:$D$514,3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P67">
+        <v>#N/A</v>
+      </c>
+      <c r="P67" t="e">
         <f ca="1">VLOOKUP(B67,actions!$A$2:$D$514,4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q67" t="b">
+        <v>#N/A</v>
+      </c>
+      <c r="Q67" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="R67" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R67" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>const uint16_t PROGMEM k_dot_2_combo[] = {KC_5, KC_3, COMBO_END};</v>
+        <v>#N/A</v>
       </c>
       <c r="S67" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v xml:space="preserve">  COMBO_k_dot_2,</v>
-      </c>
-      <c r="T67" t="str">
+        <v xml:space="preserve">  COMBO_0_0_2,</v>
+      </c>
+      <c r="T67" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v xml:space="preserve">  [COMBO_k_dot_2] = COMBO(k_dot_2_combo, KC_RGHT),</v>
-      </c>
-      <c r="U67" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U67" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -32868,7 +32857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>